<commit_message>
test: Added some validations for add asset to purchase order
test: Added some validations for add asset to purchase order

Related work items: #4255, #4351
</commit_message>
<xml_diff>
--- a/xPlannerAPI.Tests/Repositories/TestData/ProjectDefault.xlsx
+++ b/xPlannerAPI.Tests/Repositories/TestData/ProjectDefault.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\source\Workspaces\XPlanner\DEV\xPlannerAPI.Tests\Repositories\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loure\Work\xPlannerRepo\xPlannerAPI.Tests\Repositories\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70BD391-CDC1-45B5-934A-5D8C34B6AEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269DABCC-1A6E-4C9D-9034-C2B51292292D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
   <si>
     <t>Phase</t>
   </si>
@@ -521,28 +521,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="21.28515625" customWidth="1"/>
+    <col min="1" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="35.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="35.5546875" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
-    <col min="10" max="11" width="21.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
+    <col min="10" max="11" width="21.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,7 +580,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -618,7 +618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -656,7 +656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -694,7 +694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -729,7 +729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -764,7 +764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -802,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -837,6 +837,44 @@
         <v>40</v>
       </c>
       <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>101</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9">
         <v>1</v>
       </c>
     </row>
@@ -844,5 +882,6 @@
   <autoFilter ref="A1:L1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>